<commit_message>
GSA reads customer priority no.
</commit_message>
<xml_diff>
--- a/AgentProxy/resources/GSA/database/customer#1.xlsx
+++ b/AgentProxy/resources/GSA/database/customer#1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14790" windowHeight="5985"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14835" windowHeight="5985"/>
   </bookViews>
   <sheets>
     <sheet name="customer1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>j1</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>j5o5</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -397,70 +400,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="3" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>